<commit_message>
Put plants dataset into db
</commit_message>
<xml_diff>
--- a/data/questionIndices.xlsx
+++ b/data/questionIndices.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Dropbox\BIDS\EDAM\brian\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Documents\EDAM\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -567,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>